<commit_message>
added quick manufacturing cost summary
</commit_message>
<xml_diff>
--- a/Tables for Final Report.xlsx
+++ b/Tables for Final Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwnetid-my.sharepoint.com/personal/hpontes_uw_edu/Documents/485 - Final project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaoto\Desktop\School\CHEME\CHEME_485\Pontes_Ramos_Gao_Carpenter_485Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="975" documentId="13_ncr:1_{DEA9C033-49A8-4E15-8041-1F48C580095F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A5D5F757-05CD-4D7F-8B62-E048D02111CD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57DB891D-5E2A-423F-A7A4-57D50A1ED405}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{6F586CE1-B146-4EEE-B671-C5DD4E8C1978}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="7" xr2:uid="{6F586CE1-B146-4EEE-B671-C5DD4E8C1978}"/>
   </bookViews>
   <sheets>
     <sheet name="ASPEN" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,9 @@
     <sheet name="Utility Cost" sheetId="6" r:id="rId5"/>
     <sheet name="COM and Cashflow Diagrams" sheetId="8" r:id="rId6"/>
     <sheet name="Calculations" sheetId="2" r:id="rId7"/>
+    <sheet name="Manufac. Cost Summary" sheetId="9" r:id="rId8"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId8"/>
     <externalReference r:id="rId9"/>
   </externalReferences>
   <definedNames>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="213">
   <si>
     <t>6A</t>
   </si>
@@ -679,6 +679,21 @@
   </si>
   <si>
     <t>After-Tax Cash-Flow</t>
+  </si>
+  <si>
+    <t>Raw Materials Expenses</t>
+  </si>
+  <si>
+    <t>Product Sales</t>
+  </si>
+  <si>
+    <t>Utilities</t>
+  </si>
+  <si>
+    <t>Labor</t>
+  </si>
+  <si>
+    <t>Annual Cost/Profit ($/year)</t>
   </si>
 </sst>
 </file>
@@ -831,7 +846,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -946,6 +961,12 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -4371,208 +4392,6 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Prob 3"/>
-      <sheetName val="Prob 4"/>
-      <sheetName val="Prob 5"/>
-      <sheetName val="Prob 6"/>
-      <sheetName val="Prob 7"/>
-      <sheetName val="Prob 8"/>
-      <sheetName val="Prob 9"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3">
-        <row r="3">
-          <cell r="G3">
-            <v>0</v>
-          </cell>
-          <cell r="H3">
-            <v>-165</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="G4">
-            <v>1</v>
-          </cell>
-          <cell r="H4">
-            <v>30</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="G5">
-            <v>2</v>
-          </cell>
-          <cell r="H5">
-            <v>45</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="G6">
-            <v>3</v>
-          </cell>
-          <cell r="H6">
-            <v>45</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="G7">
-            <v>4</v>
-          </cell>
-          <cell r="H7">
-            <v>45</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="G8">
-            <v>5</v>
-          </cell>
-          <cell r="H8">
-            <v>45</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="G9">
-            <v>6</v>
-          </cell>
-          <cell r="H9">
-            <v>45</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="G10">
-            <v>7</v>
-          </cell>
-          <cell r="H10">
-            <v>45</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="G11">
-            <v>8</v>
-          </cell>
-          <cell r="H11">
-            <v>45</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="G12">
-            <v>9</v>
-          </cell>
-          <cell r="H12">
-            <v>45</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="G13">
-            <v>10</v>
-          </cell>
-          <cell r="H13">
-            <v>70</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19">
-            <v>0</v>
-          </cell>
-          <cell r="G19">
-            <v>-165</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20">
-            <v>1</v>
-          </cell>
-          <cell r="G20">
-            <v>43</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="A21">
-            <v>2</v>
-          </cell>
-          <cell r="G21">
-            <v>76.599999999999994</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="A22">
-            <v>3</v>
-          </cell>
-          <cell r="G22">
-            <v>56.760000000000005</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="A23">
-            <v>4</v>
-          </cell>
-          <cell r="G23">
-            <v>44.855999999999995</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="A24">
-            <v>5</v>
-          </cell>
-          <cell r="G24">
-            <v>44.855999999999995</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="A25">
-            <v>6</v>
-          </cell>
-          <cell r="G25">
-            <v>35.927999999999997</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="A26">
-            <v>7</v>
-          </cell>
-          <cell r="G26">
-            <v>27</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="A27">
-            <v>8</v>
-          </cell>
-          <cell r="G27">
-            <v>27</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="A28">
-            <v>9</v>
-          </cell>
-          <cell r="G28">
-            <v>27</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="A29">
-            <v>10</v>
-          </cell>
-          <cell r="G29">
-            <v>42</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4877,17 +4696,17 @@
       <selection pane="bottomLeft" activeCell="B8" sqref="B8:U8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="17" width="8.77734375" style="1"/>
-    <col min="18" max="18" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="17" width="8.81640625" style="1"/>
+    <col min="18" max="18" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.77734375" customWidth="1"/>
+    <col min="20" max="20" width="8.81640625" customWidth="1"/>
     <col min="21" max="21" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -4952,12 +4771,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -5022,7 +4841,7 @@
         <v>234.4</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -5087,7 +4906,7 @@
         <v>30.95</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -5152,7 +4971,7 @@
         <v>0.14399999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -5217,7 +5036,7 @@
         <v>421.86399999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -5282,7 +5101,7 @@
         <v>7600</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
@@ -5367,7 +5186,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -5432,7 +5251,7 @@
         <v>1375.57</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -5497,7 +5316,7 @@
         <v>-105.929</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -5562,7 +5381,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -5627,7 +5446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -5692,7 +5511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -5757,7 +5576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -5822,7 +5641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -5887,7 +5706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -5952,12 +5771,12 @@
         <v>421.86399999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>15</v>
       </c>
@@ -5965,7 +5784,7 @@
         <v>78.11</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
@@ -5973,7 +5792,7 @@
         <v>42.08</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
@@ -5981,7 +5800,7 @@
         <v>44.1</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>18</v>
       </c>
@@ -5989,7 +5808,7 @@
         <v>162.27000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>19</v>
       </c>
@@ -5997,7 +5816,7 @@
         <v>120.19</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -6005,12 +5824,12 @@
         <v>18.010000000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>15</v>
       </c>
@@ -6095,7 +5914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>16</v>
       </c>
@@ -6180,7 +5999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>17</v>
       </c>
@@ -6265,7 +6084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>18</v>
       </c>
@@ -6350,7 +6169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>19</v>
       </c>
@@ -6435,7 +6254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>22</v>
       </c>
@@ -6533,12 +6352,12 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="20.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.453125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:17" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B2" s="16" t="s">
         <v>47</v>
       </c>
@@ -6588,7 +6407,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
         <v>52</v>
       </c>
@@ -6638,7 +6457,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
@@ -6688,7 +6507,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B5" s="6" t="s">
         <v>48</v>
       </c>
@@ -6738,7 +6557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B6" s="6" t="s">
         <v>46</v>
       </c>
@@ -6788,7 +6607,7 @@
         <v>0.160968</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B7" s="12" t="s">
         <v>11</v>
       </c>
@@ -6838,7 +6657,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B8" s="6" t="s">
         <v>40</v>
       </c>
@@ -6888,7 +6707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B9" s="6" t="s">
         <v>41</v>
       </c>
@@ -6938,7 +6757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B10" s="6" t="s">
         <v>42</v>
       </c>
@@ -6988,7 +6807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B11" s="6" t="s">
         <v>43</v>
       </c>
@@ -7038,7 +6857,7 @@
         <v>0.99199999999999999</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B12" s="6" t="s">
         <v>44</v>
       </c>
@@ -7088,7 +6907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B13" s="13" t="s">
         <v>45</v>
       </c>
@@ -7151,13 +6970,13 @@
       <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="14" width="10.77734375" customWidth="1"/>
+    <col min="2" max="2" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="14" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" s="20" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:14" s="20" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B2" s="24" t="s">
         <v>51</v>
       </c>
@@ -7198,7 +7017,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
         <v>52</v>
       </c>
@@ -7239,7 +7058,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B4" s="6" t="s">
         <v>56</v>
       </c>
@@ -7280,7 +7099,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B5" s="13" t="s">
         <v>46</v>
       </c>
@@ -7334,12 +7153,12 @@
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="7" width="15.21875" customWidth="1"/>
+    <col min="2" max="7" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" s="20" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" s="20" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B2" s="24" t="s">
         <v>82</v>
       </c>
@@ -7359,7 +7178,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B3" s="21" t="s">
         <v>65</v>
       </c>
@@ -7379,7 +7198,7 @@
         <v>102400</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B4" s="21" t="s">
         <v>66</v>
       </c>
@@ -7399,7 +7218,7 @@
         <v>414000</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B5" s="21" t="s">
         <v>67</v>
       </c>
@@ -7419,7 +7238,7 @@
         <v>159000</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B6" s="21" t="s">
         <v>68</v>
       </c>
@@ -7439,7 +7258,7 @@
         <v>312000</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B7" s="21" t="s">
         <v>69</v>
       </c>
@@ -7459,7 +7278,7 @@
         <v>94200</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B8" s="21" t="s">
         <v>70</v>
       </c>
@@ -7479,7 +7298,7 @@
         <v>120000</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B9" s="21" t="s">
         <v>83</v>
       </c>
@@ -7499,7 +7318,7 @@
         <v>294000</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B10" s="21" t="s">
         <v>88</v>
       </c>
@@ -7519,7 +7338,7 @@
         <v>1830000</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B11" s="21" t="s">
         <v>115</v>
       </c>
@@ -7539,7 +7358,7 @@
         <v>87400</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B12" s="21" t="s">
         <v>116</v>
       </c>
@@ -7559,7 +7378,7 @@
         <v>55500</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B13" s="21" t="s">
         <v>117</v>
       </c>
@@ -7579,7 +7398,7 @@
         <v>33600</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B14" s="21" t="s">
         <v>118</v>
       </c>
@@ -7599,7 +7418,7 @@
         <v>30500</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B15" s="21" t="s">
         <v>119</v>
       </c>
@@ -7619,7 +7438,7 @@
         <v>35700</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B16" s="21" t="s">
         <v>120</v>
       </c>
@@ -7639,7 +7458,7 @@
         <v>111900</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B17" s="21" t="s">
         <v>121</v>
       </c>
@@ -7659,7 +7478,7 @@
         <v>111900</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B18" s="21" t="s">
         <v>122</v>
       </c>
@@ -7679,7 +7498,7 @@
         <v>111900</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B19" s="21" t="s">
         <v>123</v>
       </c>
@@ -7699,7 +7518,7 @@
         <v>111900</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B20" s="21" t="s">
         <v>94</v>
       </c>
@@ -7719,7 +7538,7 @@
         <v>94100</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B21" s="21" t="s">
         <v>95</v>
       </c>
@@ -7739,7 +7558,7 @@
         <v>123400</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B22" s="21" t="s">
         <v>96</v>
       </c>
@@ -7759,7 +7578,7 @@
         <v>39300</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B23" s="21" t="s">
         <v>97</v>
       </c>
@@ -7779,7 +7598,7 @@
         <v>41200</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B24" s="21" t="s">
         <v>98</v>
       </c>
@@ -7799,7 +7618,7 @@
         <v>44100</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B25" s="22" t="s">
         <v>99</v>
       </c>
@@ -7819,7 +7638,7 @@
         <v>57900</v>
       </c>
     </row>
-    <row r="26" spans="2:7" s="19" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" s="19" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="F26" s="27" t="s">
         <v>111</v>
       </c>
@@ -7842,13 +7661,13 @@
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.6640625" style="4" customWidth="1"/>
-    <col min="3" max="8" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="9.6328125" style="4" customWidth="1"/>
+    <col min="3" max="8" width="13.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" s="20" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:11" s="20" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B2" s="24" t="s">
         <v>126</v>
       </c>
@@ -7871,7 +7690,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
         <v>65</v>
       </c>
@@ -7894,7 +7713,7 @@
         <v>1798000</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B4" s="6" t="s">
         <v>66</v>
       </c>
@@ -7917,7 +7736,7 @@
         <v>56268.377</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B5" s="6" t="s">
         <v>67</v>
       </c>
@@ -7940,7 +7759,7 @@
         <v>20468.724999999999</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B6" s="6" t="s">
         <v>68</v>
       </c>
@@ -7963,7 +7782,7 @@
         <v>1003300</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B7" s="6" t="s">
         <v>69</v>
       </c>
@@ -7986,7 +7805,7 @@
         <v>17074.946</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B8" s="6" t="s">
         <v>70</v>
       </c>
@@ -8009,7 +7828,7 @@
         <v>853700</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B9" s="6" t="s">
         <v>88</v>
       </c>
@@ -8032,7 +7851,7 @@
         <v>1622700</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B10" s="6" t="s">
         <v>89</v>
       </c>
@@ -8055,7 +7874,7 @@
         <v>14700</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B11" s="6" t="s">
         <v>90</v>
       </c>
@@ -8078,7 +7897,7 @@
         <v>4560</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B12" s="6" t="s">
         <v>91</v>
       </c>
@@ -8101,7 +7920,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B13" s="6" t="s">
         <v>92</v>
       </c>
@@ -8125,7 +7944,7 @@
       </c>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B14" s="6" t="s">
         <v>93</v>
       </c>
@@ -8148,7 +7967,7 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B15" s="6" t="s">
         <v>83</v>
       </c>
@@ -8171,7 +7990,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B16" s="6" t="s">
         <v>94</v>
       </c>
@@ -8194,7 +8013,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B17" s="6" t="s">
         <v>95</v>
       </c>
@@ -8217,7 +8036,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B18" s="6" t="s">
         <v>120</v>
       </c>
@@ -8240,7 +8059,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B19" s="6" t="s">
         <v>121</v>
       </c>
@@ -8263,7 +8082,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B20" s="6" t="s">
         <v>122</v>
       </c>
@@ -8286,7 +8105,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B21" s="6" t="s">
         <v>123</v>
       </c>
@@ -8309,7 +8128,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B22" s="6" t="s">
         <v>96</v>
       </c>
@@ -8332,7 +8151,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B23" s="6" t="s">
         <v>97</v>
       </c>
@@ -8355,7 +8174,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B24" s="6" t="s">
         <v>98</v>
       </c>
@@ -8378,7 +8197,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B25" s="6" t="s">
         <v>99</v>
       </c>
@@ -8401,7 +8220,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B26" s="16" t="s">
         <v>138</v>
       </c>
@@ -8433,24 +8252,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{133EC853-2E76-46DB-912A-55261FCD859A}">
   <dimension ref="A2:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="1" max="1" width="37.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.36328125" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>126</v>
       </c>
@@ -8466,13 +8285,13 @@
       <c r="E2" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="G2" s="39" t="s">
+      <c r="G2" s="50" t="s">
         <v>142</v>
       </c>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>143</v>
       </c>
@@ -8498,7 +8317,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>148</v>
       </c>
@@ -8525,7 +8344,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>187</v>
       </c>
@@ -8552,7 +8371,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>188</v>
       </c>
@@ -8572,14 +8391,14 @@
         <v>2</v>
       </c>
       <c r="H6" s="49">
-        <f t="shared" ref="H6:H14" si="0">$C$10-$C$13</f>
+        <f t="shared" ref="H6:H13" si="0">$C$10-$C$13</f>
         <v>-8392993.4099999964</v>
       </c>
       <c r="I6" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>189</v>
       </c>
@@ -8606,7 +8425,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>150</v>
       </c>
@@ -8634,7 +8453,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>185</v>
       </c>
@@ -8662,7 +8481,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>200</v>
       </c>
@@ -8689,7 +8508,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>153</v>
       </c>
@@ -8716,7 +8535,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>190</v>
       </c>
@@ -8743,7 +8562,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>199</v>
       </c>
@@ -8768,7 +8587,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>173</v>
       </c>
@@ -8795,7 +8614,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>140</v>
       </c>
@@ -8809,7 +8628,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>172</v>
       </c>
@@ -8823,7 +8642,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>176</v>
       </c>
@@ -8837,7 +8656,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>139</v>
       </c>
@@ -8845,7 +8664,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>161</v>
       </c>
@@ -8862,7 +8681,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A21" s="42" t="s">
         <v>145</v>
       </c>
@@ -8892,7 +8711,7 @@
       </c>
       <c r="J21" s="42"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="19">
         <v>0</v>
       </c>
@@ -8918,7 +8737,7 @@
       </c>
       <c r="J22" s="42"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>1</v>
       </c>
@@ -8955,7 +8774,7 @@
       </c>
       <c r="J23" s="44"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2</v>
       </c>
@@ -8992,7 +8811,7 @@
       </c>
       <c r="J24" s="44"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>3</v>
       </c>
@@ -9029,7 +8848,7 @@
       </c>
       <c r="J25" s="44"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>4</v>
       </c>
@@ -9066,7 +8885,7 @@
       </c>
       <c r="J26" s="44"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>5</v>
       </c>
@@ -9103,7 +8922,7 @@
       </c>
       <c r="J27" s="44"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>6</v>
       </c>
@@ -9140,7 +8959,7 @@
       </c>
       <c r="J28" s="44"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>7</v>
       </c>
@@ -9176,7 +8995,7 @@
         <v>-25092400.015499987</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>8</v>
       </c>
@@ -9212,7 +9031,7 @@
         <v>-26972845.731999986</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>9</v>
       </c>
@@ -9248,7 +9067,7 @@
         <v>-28853291.448499985</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>10</v>
       </c>
@@ -9284,7 +9103,7 @@
         <v>-30733737.164999984</v>
       </c>
     </row>
-    <row r="34" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E34" s="5" t="s">
         <v>157</v>
       </c>
@@ -9295,7 +9114,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="35" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E35" s="45">
         <v>0.09</v>
       </c>
@@ -9325,55 +9144,55 @@
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6328125" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="39" t="s">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="39" t="s">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A3" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39" t="s">
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39" t="s">
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
       <c r="L3" s="3" t="s">
         <v>33</v>
       </c>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -9417,7 +9236,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -9467,7 +9286,7 @@
         <v>0.16431703478668797</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -9515,7 +9334,7 @@
         <v>0.81547823169822575</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G8" t="s">
         <v>80</v>
       </c>
@@ -9529,7 +9348,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -9549,7 +9368,7 @@
         <v>1.4800000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9840</v>
       </c>
@@ -9557,7 +9376,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>64</v>
       </c>
@@ -9580,7 +9399,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>65</v>
       </c>
@@ -9609,7 +9428,7 @@
         <v>7.2052052052052042</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>66</v>
       </c>
@@ -9639,7 +9458,7 @@
         <v>456.85135135135135</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>67</v>
       </c>
@@ -9669,7 +9488,7 @@
         <v>166.18864864864867</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -9698,7 +9517,7 @@
         <v>4.2605086541858004</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>69</v>
       </c>
@@ -9728,7 +9547,7 @@
         <v>138.63405405405405</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -9767,4 +9586,66 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F6BCBF7-C87F-4D83-A22D-5F338F8C4C7B}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.26953125" style="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7265625" style="39" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B1" s="39" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="39" t="s">
+        <v>208</v>
+      </c>
+      <c r="B2" s="51">
+        <v>-116408517</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="39" t="s">
+        <v>209</v>
+      </c>
+      <c r="B3" s="51">
+        <v>144137412</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="39" t="s">
+        <v>210</v>
+      </c>
+      <c r="B4" s="51">
+        <v>-5210000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="39" t="s">
+        <v>211</v>
+      </c>
+      <c r="B5" s="51">
+        <v>-834120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B6" s="51">
+        <f>SUM(B2:B5)</f>
+        <v>21684775</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>